<commit_message>
Paper versión (ya no sé)
</commit_message>
<xml_diff>
--- a/Análisis estadístico/Kaplan_Meier/120_días/Estimación_críticos/Edad/Outcome_g2.xlsx
+++ b/Análisis estadístico/Kaplan_Meier/120_días/Estimación_críticos/Edad/Outcome_g2.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -399,22 +399,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>576</v>
+        <v>609</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>104</v>
       </c>
       <c r="D2">
-        <v>0.953125</v>
+        <v>0.8292282430213465</v>
       </c>
       <c r="E2">
-        <v>0.009240265886932161</v>
+        <v>0.01838917874749263</v>
       </c>
       <c r="F2">
-        <v>0.9242068146697793</v>
+        <v>0.7857184410281751</v>
       </c>
       <c r="G2">
-        <v>0.971180818345442</v>
+        <v>0.8646689923577622</v>
       </c>
     </row>
     <row r="3">
@@ -422,22 +422,22 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>424</v>
+        <v>502</v>
       </c>
       <c r="C3">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D3">
-        <v>0.8991745283018868</v>
+        <v>0.7730653739720919</v>
       </c>
       <c r="E3">
-        <v>0.01506293290244189</v>
+        <v>0.02197457984238632</v>
       </c>
       <c r="F3">
-        <v>0.8580381682770483</v>
+        <v>0.7256404713767705</v>
       </c>
       <c r="G3">
-        <v>0.9288831322588569</v>
+        <v>0.8133608431841807</v>
       </c>
     </row>
     <row r="4">
@@ -445,22 +445,22 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>386</v>
+        <v>467</v>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D4">
-        <v>0.8223020945351452</v>
+        <v>0.7349914904574063</v>
       </c>
       <c r="E4">
-        <v>0.02165824467254058</v>
+        <v>0.0243681511070357</v>
       </c>
       <c r="F4">
-        <v>0.7708955930003389</v>
+        <v>0.6855591986977431</v>
       </c>
       <c r="G4">
-        <v>0.8632004944866263</v>
+        <v>0.777934706506681</v>
       </c>
     </row>
     <row r="5">
@@ -468,22 +468,22 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>337</v>
+        <v>441</v>
       </c>
       <c r="C5">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D5">
-        <v>0.7417799309753239</v>
+        <v>0.68999201144981</v>
       </c>
       <c r="E5">
-        <v>0.02812817441749562</v>
+        <v>0.02723402337937361</v>
       </c>
       <c r="F5">
-        <v>0.6833836058631323</v>
+        <v>0.6387164826710087</v>
       </c>
       <c r="G5">
-        <v>0.7910714009006464</v>
+        <v>0.7355350804965715</v>
       </c>
     </row>
     <row r="6">
@@ -491,22 +491,22 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>295</v>
+        <v>414</v>
       </c>
       <c r="C6">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D6">
-        <v>0.6940042744040319</v>
+        <v>0.6399925903302586</v>
       </c>
       <c r="E6">
-        <v>0.03200862529668495</v>
+        <v>0.03050245496508219</v>
       </c>
       <c r="F6">
-        <v>0.6326914911417323</v>
+        <v>0.5873067421540219</v>
       </c>
       <c r="G6">
-        <v>0.7471636187681197</v>
+        <v>0.6878002163852286</v>
       </c>
     </row>
     <row r="7">
@@ -514,22 +514,22 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>267</v>
+        <v>382</v>
       </c>
       <c r="C7">
         <v>14</v>
       </c>
       <c r="D7">
-        <v>0.6576145371693636</v>
+        <v>0.6165373645066365</v>
       </c>
       <c r="E7">
-        <v>0.03509704989431632</v>
+        <v>0.03209345752835419</v>
       </c>
       <c r="F7">
-        <v>0.5945024303697187</v>
+        <v>0.5633866793898933</v>
       </c>
       <c r="G7">
-        <v>0.7133256397386714</v>
+        <v>0.6652128138848299</v>
       </c>
     </row>
     <row r="8">
@@ -537,22 +537,22 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>248</v>
+        <v>366</v>
       </c>
       <c r="C8">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D8">
-        <v>0.5727610485023489</v>
+        <v>0.5929539680500985</v>
       </c>
       <c r="E8">
-        <v>0.04276884936957773</v>
+        <v>0.03374401680112928</v>
       </c>
       <c r="F8">
-        <v>0.5070756105632628</v>
+        <v>0.5394512436076043</v>
       </c>
       <c r="G8">
-        <v>0.6329734351429654</v>
+        <v>0.642388019005476</v>
       </c>
     </row>
     <row r="9">
@@ -560,22 +560,22 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>206</v>
+        <v>350</v>
       </c>
       <c r="C9">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D9">
-        <v>0.5254943600337084</v>
+        <v>0.5455176506060906</v>
       </c>
       <c r="E9">
-        <v>0.04760053398192173</v>
+        <v>0.03724387029893429</v>
       </c>
       <c r="F9">
-        <v>0.4590996426491824</v>
+        <v>0.4916617746988764</v>
       </c>
       <c r="G9">
-        <v>0.5875585113940891</v>
+        <v>0.596131384396811</v>
       </c>
     </row>
     <row r="10">
@@ -583,22 +583,22 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>178</v>
+        <v>321</v>
       </c>
       <c r="C10">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10">
-        <v>0.4812111274465982</v>
+        <v>0.5217256035391583</v>
       </c>
       <c r="E10">
-        <v>0.05275227608764926</v>
+        <v>0.0391046041734738</v>
       </c>
       <c r="F10">
-        <v>0.41446343772432</v>
+        <v>0.4678741655483216</v>
       </c>
       <c r="G10">
-        <v>0.5447419921888105</v>
+        <v>0.5727553605096475</v>
       </c>
     </row>
     <row r="11">
@@ -606,22 +606,22 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>151</v>
+        <v>307</v>
       </c>
       <c r="C11">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D11">
-        <v>0.4525296695193175</v>
+        <v>0.5013324203389307</v>
       </c>
       <c r="E11">
-        <v>0.05659098512363027</v>
+        <v>0.04076360614335571</v>
       </c>
       <c r="F11">
-        <v>0.3856094688966996</v>
+        <v>0.4475844521648638</v>
       </c>
       <c r="G11">
-        <v>0.5169817412518284</v>
+        <v>0.5526228225386416</v>
       </c>
     </row>
     <row r="12">
@@ -629,22 +629,22 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>137</v>
+        <v>294</v>
       </c>
       <c r="C12">
         <v>9</v>
       </c>
       <c r="D12">
-        <v>0.4228014430545448</v>
+        <v>0.4859855095122287</v>
       </c>
       <c r="E12">
-        <v>0.0609571121713475</v>
+        <v>0.04206046803612035</v>
       </c>
       <c r="F12">
-        <v>0.355902347703537</v>
+        <v>0.4323701509505377</v>
       </c>
       <c r="G12">
-        <v>0.4880562700331886</v>
+        <v>0.5374191128595568</v>
       </c>
     </row>
     <row r="13">
@@ -652,22 +652,22 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>117</v>
+        <v>284</v>
       </c>
       <c r="C13">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D13">
-        <v>0.3830508800323226</v>
+        <v>0.4757182100154915</v>
       </c>
       <c r="E13">
-        <v>0.06784337286288646</v>
+        <v>0.04295437711121412</v>
       </c>
       <c r="F13">
-        <v>0.31623668841015</v>
+        <v>0.4222167902352601</v>
       </c>
       <c r="G13">
-        <v>0.4494083511173014</v>
+        <v>0.5272232610608506</v>
       </c>
     </row>
     <row r="14">
@@ -675,22 +675,22 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>97</v>
+        <v>277</v>
       </c>
       <c r="C14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>0.3475100767303546</v>
+        <v>0.4585442674156542</v>
       </c>
       <c r="E14">
-        <v>0.07521357094656216</v>
+        <v>0.0445004332768033</v>
       </c>
       <c r="F14">
-        <v>0.2809464879681264</v>
+        <v>0.4052795550403477</v>
       </c>
       <c r="G14">
-        <v>0.4148065252267289</v>
+        <v>0.5101244985926427</v>
       </c>
     </row>
     <row r="15">
@@ -698,22 +698,22 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>80</v>
+        <v>265</v>
       </c>
       <c r="C15">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D15">
-        <v>0.3084151930981897</v>
+        <v>0.4464317773329766</v>
       </c>
       <c r="E15">
-        <v>0.08509752227172691</v>
+        <v>0.04563630844416436</v>
       </c>
       <c r="F15">
-        <v>0.2423777404935946</v>
+        <v>0.3933643196736057</v>
       </c>
       <c r="G15">
-        <v>0.3766936721293259</v>
+        <v>0.4980359558098534</v>
       </c>
     </row>
     <row r="16">
@@ -721,22 +721,22 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="C16">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D16">
-        <v>0.2643558797984483</v>
+        <v>0.4342721569386931</v>
       </c>
       <c r="E16">
-        <v>0.09943385209419227</v>
+        <v>0.04681476332048812</v>
       </c>
       <c r="F16">
-        <v>0.1993091976190085</v>
+        <v>0.3814317811039237</v>
       </c>
       <c r="G16">
-        <v>0.3337113689870965</v>
+        <v>0.4858727354274412</v>
       </c>
     </row>
     <row r="17">
@@ -744,22 +744,22 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>51</v>
+        <v>249</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>0.2591724311749493</v>
+        <v>0.4290399622767812</v>
       </c>
       <c r="E17">
-        <v>0.1013866253755139</v>
+        <v>0.04733496021052211</v>
       </c>
       <c r="F17">
-        <v>0.1942942725895851</v>
+        <v>0.3763056659281752</v>
       </c>
       <c r="G17">
-        <v>0.3286343201948242</v>
+        <v>0.480631063964808</v>
       </c>
     </row>
     <row r="18">
@@ -767,22 +767,22 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>41</v>
+        <v>246</v>
       </c>
       <c r="C18">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>0.2086022007017884</v>
+        <v>0.4238077676148692</v>
       </c>
       <c r="E18">
-        <v>0.1272479241702044</v>
+        <v>0.04786213686384851</v>
       </c>
       <c r="F18">
-        <v>0.1448745530958912</v>
+        <v>0.3711860678646715</v>
       </c>
       <c r="G18">
-        <v>0.2803937117670425</v>
+        <v>0.4753832175327872</v>
       </c>
     </row>
     <row r="19">
@@ -790,22 +790,22 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>27</v>
+        <v>242</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D19">
-        <v>0.1854241784015897</v>
+        <v>0.4080463217118369</v>
       </c>
       <c r="E19">
-        <v>0.1442971373079026</v>
+        <v>0.04950149728823686</v>
       </c>
       <c r="F19">
-        <v>0.1223373459297591</v>
+        <v>0.3557964218329365</v>
       </c>
       <c r="G19">
-        <v>0.2588358984953177</v>
+        <v>0.4595438735907797</v>
       </c>
     </row>
     <row r="20">
@@ -813,22 +813,22 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>14</v>
+        <v>233</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>0.105956673372337</v>
+        <v>0.4045437781778297</v>
       </c>
       <c r="E20">
-        <v>0.2727509714129068</v>
+        <v>0.04987541547916587</v>
       </c>
       <c r="F20">
-        <v>0.04643710454334611</v>
+        <v>0.3523847083182514</v>
       </c>
       <c r="G20">
-        <v>0.1936924912148931</v>
+        <v>0.4560162550464553</v>
       </c>
     </row>
     <row r="21">
@@ -836,45 +836,551 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>231</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>0.08829722781028082</v>
+        <v>0.3975386911098154</v>
       </c>
       <c r="E21">
-        <v>0.3282170405996886</v>
+        <v>0.05063436662808594</v>
       </c>
       <c r="F21">
-        <v>0.0321153387726919</v>
+        <v>0.3455703040650194</v>
       </c>
       <c r="G21">
-        <v>0.1802957446065589</v>
+        <v>0.4489524787505041</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>120</v>
+        <v>21</v>
       </c>
       <c r="B22">
+        <v>227</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>0.3922848758088046</v>
+      </c>
+      <c r="E22">
+        <v>0.0512136549613558</v>
+      </c>
+      <c r="F22">
+        <v>0.3404674369189127</v>
+      </c>
+      <c r="G22">
+        <v>0.4436471339746236</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>223</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>0.38348925079067</v>
+      </c>
+      <c r="E23">
+        <v>0.05220813619607704</v>
+      </c>
+      <c r="F23">
+        <v>0.3319355363571397</v>
+      </c>
+      <c r="G23">
+        <v>0.4347549934248834</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>217</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>0.3746530929383504</v>
+      </c>
+      <c r="E24">
+        <v>0.05323885504279769</v>
+      </c>
+      <c r="F24">
+        <v>0.3233795486318419</v>
+      </c>
+      <c r="G24">
+        <v>0.4258077146545598</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>212</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>0.3658169350860307</v>
+      </c>
+      <c r="E25">
+        <v>0.05429836487951261</v>
+      </c>
+      <c r="F25">
+        <v>0.3148437503490229</v>
+      </c>
+      <c r="G25">
+        <v>0.4168414017176276</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>207</v>
+      </c>
+      <c r="C26">
         <v>1</v>
       </c>
-      <c r="C22">
+      <c r="D26">
+        <v>0.3640497035155668</v>
+      </c>
+      <c r="E26">
+        <v>0.05451388342643907</v>
+      </c>
+      <c r="F26">
+        <v>0.3131390346447047</v>
+      </c>
+      <c r="G26">
+        <v>0.4150458342316802</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>206</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>0.360515240374639</v>
+      </c>
+      <c r="E27">
+        <v>0.05494866093460585</v>
+      </c>
+      <c r="F27">
+        <v>0.3097320637961242</v>
+      </c>
+      <c r="G27">
+        <v>0.4114523781694794</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>204</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>0.3534463140927833</v>
+      </c>
+      <c r="E28">
+        <v>0.05583363282281167</v>
+      </c>
+      <c r="F28">
+        <v>0.3029280264105791</v>
+      </c>
+      <c r="G28">
+        <v>0.4042561214301822</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>198</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>0.3498761493039673</v>
+      </c>
+      <c r="E29">
+        <v>0.05629325288179778</v>
+      </c>
+      <c r="F29">
+        <v>0.2994926464991277</v>
+      </c>
+      <c r="G29">
+        <v>0.400620990922391</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>195</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>0.3462876759777728</v>
+      </c>
+      <c r="E30">
+        <v>0.05676330101454612</v>
+      </c>
+      <c r="F30">
+        <v>0.2960410844380186</v>
+      </c>
+      <c r="G30">
+        <v>0.3969660362087153</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>193</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>0.3426992026515783</v>
+      </c>
+      <c r="E31">
+        <v>0.05723921108863873</v>
+      </c>
+      <c r="F31">
+        <v>0.2925931188875295</v>
+      </c>
+      <c r="G31">
+        <v>0.3933077128825233</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>191</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0.340904965988481</v>
+      </c>
+      <c r="E32">
+        <v>0.05747941445896738</v>
+      </c>
+      <c r="F32">
+        <v>0.2908704915301992</v>
+      </c>
+      <c r="G32">
+        <v>0.3914772813969943</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>190</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0.3391107293253838</v>
+      </c>
+      <c r="E33">
+        <v>0.05772114415718209</v>
+      </c>
+      <c r="F33">
+        <v>0.2891487714910431</v>
+      </c>
+      <c r="G33">
+        <v>0.3896459997395854</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>188</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>0.3355031683751137</v>
+      </c>
+      <c r="E34">
+        <v>0.05821447957910033</v>
+      </c>
+      <c r="F34">
+        <v>0.2856875787542535</v>
+      </c>
+      <c r="G34">
+        <v>0.3859636227795534</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>186</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>0.3300918269497087</v>
+      </c>
+      <c r="E35">
+        <v>0.05896662124423379</v>
+      </c>
+      <c r="F35">
+        <v>0.2805028239299288</v>
+      </c>
+      <c r="G35">
+        <v>0.3804334805259849</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>183</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>0.3282880464745737</v>
+      </c>
+      <c r="E36">
+        <v>0.05922066397085968</v>
+      </c>
+      <c r="F36">
+        <v>0.2787764605394911</v>
+      </c>
+      <c r="G36">
+        <v>0.378588333838808</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>182</v>
+      </c>
+      <c r="C37">
         <v>0</v>
       </c>
-      <c r="D22">
-        <v>0.08829722781028082</v>
-      </c>
-      <c r="E22">
-        <v>0.3282170405996886</v>
-      </c>
-      <c r="F22">
-        <v>0.0321153387726919</v>
-      </c>
-      <c r="G22">
-        <v>0.1802957446065589</v>
+      <c r="D37">
+        <v>0.3282880464745737</v>
+      </c>
+      <c r="E37">
+        <v>0.05922066397085968</v>
+      </c>
+      <c r="F37">
+        <v>0.2787764605394911</v>
+      </c>
+      <c r="G37">
+        <v>0.378588333838808</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>181</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>0.3264743003614545</v>
+      </c>
+      <c r="E38">
+        <v>0.05947924611368233</v>
+      </c>
+      <c r="F38">
+        <v>0.2770403565149021</v>
+      </c>
+      <c r="G38">
+        <v>0.3767332971662641</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>180</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>0.3246605542483353</v>
+      </c>
+      <c r="E39">
+        <v>0.05973957935462376</v>
+      </c>
+      <c r="F39">
+        <v>0.2753052277792918</v>
+      </c>
+      <c r="G39">
+        <v>0.3748773504518514</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>179</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0.3228468081352161</v>
+      </c>
+      <c r="E40">
+        <v>0.06000168906611152</v>
+      </c>
+      <c r="F40">
+        <v>0.2735710777412514</v>
+      </c>
+      <c r="G40">
+        <v>0.3730204903673732</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>178</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>0.3192193159089777</v>
+      </c>
+      <c r="E41">
+        <v>0.06053134183639598</v>
+      </c>
+      <c r="F41">
+        <v>0.2701057277615219</v>
+      </c>
+      <c r="G41">
+        <v>0.3693040164410399</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>176</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>0.3174055697958585</v>
+      </c>
+      <c r="E42">
+        <v>0.06079893812380405</v>
+      </c>
+      <c r="F42">
+        <v>0.2683745350096424</v>
+      </c>
+      <c r="G42">
+        <v>0.3674443956052252</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>174</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>0.3137572299131475</v>
+      </c>
+      <c r="E43">
+        <v>0.06134605063549436</v>
+      </c>
+      <c r="F43">
+        <v>0.2648928285590137</v>
+      </c>
+      <c r="G43">
+        <v>0.3637035107441774</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>90</v>
+      </c>
+      <c r="B44">
+        <v>172</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0.3137572299131475</v>
+      </c>
+      <c r="E44">
+        <v>0.06134605063549436</v>
+      </c>
+      <c r="F44">
+        <v>0.2648928285590137</v>
+      </c>
+      <c r="G44">
+        <v>0.3637035107441774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>